<commit_message>
1. quick running adjustment 2. added verbosity
</commit_message>
<xml_diff>
--- a/model2/models/results.xlsx
+++ b/model2/models/results.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="16">
   <si>
     <t xml:space="preserve">Additional data</t>
   </si>
@@ -61,13 +61,13 @@
     <t xml:space="preserve">Full group</t>
   </si>
   <si>
+    <t xml:space="preserve">Minus 20 examples</t>
+  </si>
+  <si>
     <t xml:space="preserve">acc – model by loss</t>
   </si>
   <si>
     <t xml:space="preserve">AUC – model by loss</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Minus 20 examples</t>
   </si>
 </sst>
 </file>
@@ -296,14 +296,14 @@
   <dimension ref="A1:E59"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="true" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C41" activeCellId="0" sqref="C41"/>
+      <selection pane="topLeft" activeCell="C62" activeCellId="0" sqref="C62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="22.84"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="9.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="19.8"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="22.78"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="16.47"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="20.68"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="9.79"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="20.31"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="18.15"/>
@@ -398,11 +398,11 @@
       <c r="C7" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="D7" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E7" s="3" t="s">
-        <v>8</v>
+      <c r="D7" s="3" t="n">
+        <v>86</v>
+      </c>
+      <c r="E7" s="3" t="n">
+        <v>84</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -415,23 +415,23 @@
       <c r="C8" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="D8" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E8" s="3" t="s">
-        <v>8</v>
+      <c r="D8" s="3" t="n">
+        <v>86</v>
+      </c>
+      <c r="E8" s="3" t="n">
+        <v>78</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
-        <v>0</v>
+        <v>13</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="2" t="s">
-        <v>13</v>
+        <v>1</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -456,10 +456,10 @@
         <v>7</v>
       </c>
       <c r="B14" s="3" t="n">
-        <v>72</v>
+        <v>82</v>
       </c>
       <c r="C14" s="3" t="n">
-        <v>78</v>
+        <v>89</v>
       </c>
       <c r="D14" s="3" t="s">
         <v>8</v>
@@ -476,7 +476,7 @@
         <v>79</v>
       </c>
       <c r="C15" s="3" t="n">
-        <v>84</v>
+        <v>73</v>
       </c>
       <c r="D15" s="3" t="s">
         <v>8</v>
@@ -490,7 +490,7 @@
         <v>10</v>
       </c>
       <c r="B16" s="3" t="n">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C16" s="3" t="n">
         <v>73</v>
@@ -499,7 +499,7 @@
         <v>86</v>
       </c>
       <c r="E16" s="3" t="n">
-        <v>78</v>
+        <v>73</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -512,11 +512,11 @@
       <c r="C17" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="D17" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E17" s="3" t="s">
-        <v>8</v>
+      <c r="D17" s="3" t="n">
+        <v>79</v>
+      </c>
+      <c r="E17" s="3" t="n">
+        <v>73</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -529,11 +529,11 @@
       <c r="C18" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="D18" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E18" s="3" t="s">
-        <v>8</v>
+      <c r="D18" s="3" t="n">
+        <v>79</v>
+      </c>
+      <c r="E18" s="3" t="n">
+        <v>78</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -570,10 +570,10 @@
         <v>7</v>
       </c>
       <c r="B24" s="3" t="n">
-        <v>28</v>
+        <v>72</v>
       </c>
       <c r="C24" s="3" t="n">
-        <v>44</v>
+        <v>78</v>
       </c>
       <c r="D24" s="3" t="s">
         <v>8</v>
@@ -587,10 +587,10 @@
         <v>9</v>
       </c>
       <c r="B25" s="3" t="n">
-        <v>24</v>
+        <v>79</v>
       </c>
       <c r="C25" s="3" t="n">
-        <v>30</v>
+        <v>84</v>
       </c>
       <c r="D25" s="3" t="s">
         <v>8</v>
@@ -604,16 +604,16 @@
         <v>10</v>
       </c>
       <c r="B26" s="3" t="n">
-        <v>32</v>
+        <v>77</v>
       </c>
       <c r="C26" s="3" t="n">
-        <v>36</v>
+        <v>73</v>
       </c>
       <c r="D26" s="3" t="n">
-        <v>35</v>
+        <v>86</v>
       </c>
       <c r="E26" s="3" t="n">
-        <v>47</v>
+        <v>78</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -626,11 +626,11 @@
       <c r="C27" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="D27" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E27" s="3" t="s">
-        <v>8</v>
+      <c r="D27" s="3" t="n">
+        <v>79</v>
+      </c>
+      <c r="E27" s="3" t="n">
+        <v>73</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -643,23 +643,23 @@
       <c r="C28" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="D28" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E28" s="3" t="s">
-        <v>8</v>
+      <c r="D28" s="3" t="n">
+        <v>82</v>
+      </c>
+      <c r="E28" s="3" t="n">
+        <v>78</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="2" t="s">
-        <v>1</v>
+        <v>14</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -684,7 +684,7 @@
         <v>7</v>
       </c>
       <c r="B34" s="3" t="n">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="C34" s="3" t="n">
         <v>89</v>
@@ -701,7 +701,7 @@
         <v>9</v>
       </c>
       <c r="B35" s="3" t="n">
-        <v>79</v>
+        <v>68</v>
       </c>
       <c r="C35" s="3" t="n">
         <v>73</v>
@@ -718,13 +718,13 @@
         <v>10</v>
       </c>
       <c r="B36" s="3" t="n">
+        <v>68</v>
+      </c>
+      <c r="C36" s="3" t="n">
+        <v>60</v>
+      </c>
+      <c r="D36" s="3" t="n">
         <v>75</v>
-      </c>
-      <c r="C36" s="3" t="n">
-        <v>73</v>
-      </c>
-      <c r="D36" s="3" t="n">
-        <v>86</v>
       </c>
       <c r="E36" s="3" t="n">
         <v>73</v>
@@ -740,11 +740,11 @@
       <c r="C37" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="D37" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E37" s="3" t="s">
-        <v>8</v>
+      <c r="D37" s="3" t="n">
+        <v>68</v>
+      </c>
+      <c r="E37" s="3" t="n">
+        <v>68</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -757,23 +757,23 @@
       <c r="C38" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="D38" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E38" s="3" t="s">
-        <v>8</v>
+      <c r="D38" s="3" t="n">
+        <v>72</v>
+      </c>
+      <c r="E38" s="3" t="n">
+        <v>73</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="1" t="s">
-        <v>15</v>
+        <v>0</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="2" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -798,10 +798,10 @@
         <v>7</v>
       </c>
       <c r="B44" s="3" t="n">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="C44" s="3" t="n">
-        <v>89</v>
+        <v>76</v>
       </c>
       <c r="D44" s="3" t="s">
         <v>8</v>
@@ -815,10 +815,10 @@
         <v>9</v>
       </c>
       <c r="B45" s="3" t="n">
-        <v>68</v>
+        <v>76</v>
       </c>
       <c r="C45" s="3" t="n">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="D45" s="3" t="s">
         <v>8</v>
@@ -832,16 +832,16 @@
         <v>10</v>
       </c>
       <c r="B46" s="3" t="n">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="C46" s="3" t="n">
-        <v>60</v>
+        <v>78</v>
       </c>
       <c r="D46" s="3" t="n">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="E46" s="3" t="n">
-        <v>73</v>
+        <v>64</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -854,11 +854,11 @@
       <c r="C47" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="D47" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E47" s="3" t="s">
-        <v>8</v>
+      <c r="D47" s="3" t="n">
+        <v>77</v>
+      </c>
+      <c r="E47" s="3" t="n">
+        <v>81</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -871,23 +871,23 @@
       <c r="C48" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="D48" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E48" s="3" t="s">
-        <v>8</v>
+      <c r="D48" s="3" t="n">
+        <v>84</v>
+      </c>
+      <c r="E48" s="3" t="n">
+        <v>75</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -912,10 +912,10 @@
         <v>7</v>
       </c>
       <c r="B54" s="3" t="n">
-        <v>32</v>
+        <v>70</v>
       </c>
       <c r="C54" s="3" t="n">
-        <v>42</v>
+        <v>58</v>
       </c>
       <c r="D54" s="3" t="s">
         <v>8</v>
@@ -929,10 +929,10 @@
         <v>9</v>
       </c>
       <c r="B55" s="3" t="n">
-        <v>35</v>
+        <v>64</v>
       </c>
       <c r="C55" s="3" t="n">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="D55" s="3" t="s">
         <v>8</v>
@@ -946,16 +946,16 @@
         <v>10</v>
       </c>
       <c r="B56" s="3" t="n">
-        <v>29</v>
+        <v>69</v>
       </c>
       <c r="C56" s="3" t="n">
-        <v>35</v>
+        <v>61</v>
       </c>
       <c r="D56" s="3" t="n">
-        <v>36</v>
+        <v>62</v>
       </c>
       <c r="E56" s="3" t="n">
-        <v>31</v>
+        <v>70</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -968,11 +968,11 @@
       <c r="C57" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="D57" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E57" s="3" t="s">
-        <v>8</v>
+      <c r="D57" s="3" t="n">
+        <v>77</v>
+      </c>
+      <c r="E57" s="3" t="n">
+        <v>67</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -985,17 +985,34 @@
       <c r="C58" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="D58" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E58" s="3" t="s">
-        <v>8</v>
+      <c r="D58" s="3" t="n">
+        <v>80</v>
+      </c>
+      <c r="E58" s="3" t="n">
+        <v>60</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="60" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="61" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="62" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="63" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="64" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="65" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="66" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="67" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="68" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="69" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="70" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="71" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="72" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="73" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="74" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="75" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="76" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="77" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="78" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="79" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>